<commit_message>
Update load test data
</commit_message>
<xml_diff>
--- a/src/test/data/LoadCommandTest/validFlashCardFile.xlsx
+++ b/src/test/data/LoadCommandTest/validFlashCardFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiali_yu/Desktop/nus/Java/tp/src/test/data/LoadCommandTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2125C36-2CD3-E542-84EA-FAFF35DED9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B897E7-73D0-524C-B345-8E909F06D6A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="14400" xr2:uid="{9ECF4D80-8954-1545-B614-6F96ABBF09E5}"/>
   </bookViews>
@@ -36,31 +36,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Amy</t>
   </si>
   <si>
     <t>艾米</t>
   </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>鲍勃</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="Menlo-Regular"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,8 +89,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,28 +407,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034C8304-7A85-714B-BA7C-D724FFB3ECBB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>